<commit_message>
correction to instance and average hour pair
</commit_message>
<xml_diff>
--- a/CloudSQL_pricing_summary.xlsx
+++ b/CloudSQL_pricing_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,35 +516,65 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>Days/Month.1</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Zonal/Regional</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>HDD</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>SSD</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Balanced SSD</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Snapshot</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
           <t>Error</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>SUD Price</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>SUD URL</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>One Year Price</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>One Year URL</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>three Year Price</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>three Year URL</t>
         </is>
@@ -560,7 +590,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1.02</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -570,14 +600,14 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>custom</t>
+          <t>standard</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>26</v>
+        <v>3.75</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -586,11 +616,11 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>asia-south1</t>
+          <t>asia-southeast1</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>11</v>
+        <v>500</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -598,42 +628,56 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>5</v>
+        <v>250</v>
       </c>
       <c r="N2" t="n">
-        <v>730</v>
-      </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
+        <v>500</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>hours</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
       <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>$312.05</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrT0RnNVpXSXlaaTFrTWpjd0xUUmhNRE10WW1Nd05TMDJNemhpTmpreE5HUTBaVEFRQVE9PRAHGiQ4NzNCOTc0Qi0zMkI2LTQ4QkEtQkIzRi0wRkQ3MEJENTNGOEI</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>$234.46</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1WkRBek1UUXlOQzB6WkdZMkxUUTBaV0l0WWpaa015MDRPREV6TUdNMU1qZGtNV1VRQVE9PRAHGiQ0RTQ5QzZBQS00M0FGLTQzQzYtQjU5Qy0yQjQ0MUZERjg1MTc</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>$150.67</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJsTVdRNFpXSTFaaTFpTUdKaUxUUmlObVV0WWprM01DMWpOMkpqTUdNMU1XVTRNR1VRQVE9PRAHGiQ3RDE0REY0Ny1ERTUwLTQ4MTQtOUJBNC1DMTJGRTBDRDE1REU</t>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>$109.60</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVF3TkdGa09UYzNNQzA0WVRrM0xUUXpaR1l0T0RFeU55MDFOemN4WVRNNE5HVmlOalFRQVE9PRAHGiRBMEIwM0Q0Mi1DNjYyLTRFOTgtQUJFQi0xNEY5Q0ZGMjZDQzQ</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>$109.60</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVF5WkdWaVl6RmpaQzFrWXpnd0xUUTRZV1l0WW1ObU5pMDRObVJsTWpBM01tUXhaakFRQVE9PRAHGiRFREZGN0EwNi0yQThGLTQ5M0EtODkwNS0zMjA0MkExNEE4QjA</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>$109.60</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVF6TW1GaE1qZG1PQzFtTVdObExUUmlNRE10WVRBellTMHhaRE15TjJObE9ESXhNamdRQVE9PRAHGiQzNzBDNjVFOS00RDE0LTQxQzctOTdDNS03RDY5OTMyNUJBRjk</t>
         </is>
       </c>
     </row>
@@ -643,7 +687,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MySQL</t>
+          <t>PostgreSQL</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -657,442 +701,76 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>STANDARD</t>
+          <t>custom</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="H3" t="n">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>HA</t>
+          <t>Non-HA</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>asia-southeast1</t>
+          <t>us-central1</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>11</v>
+        <v>1000</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>HDD</t>
+          <t>SSD</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="N3" t="n">
-        <v>600</v>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>hours</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>month</t>
-        </is>
-      </c>
+        <v>730</v>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>$456.58</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrT0RnNVpXSXlaaTFrTWpjd0xUUmhNRE10WW1Nd05TMDJNemhpTmpreE5HUTBaVEFRQVE9PRAHGiQ5NDE4ODBFNC04REIxLTQ3MUQtODM4NS0wQkQ2ODlGNTUzRTE</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>$456.58</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1WkRBek1UUXlOQzB6WkdZMkxUUTBaV0l0WWpaa015MDRPREV6TUdNMU1qZGtNV1VRQVE9PRAHGiQzRDEwQUY5QS03RDdBLTREQzktODY5NC0yRTM5REQxQ0NGRUQ</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>$456.58</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJsTVdRNFpXSTFaaTFpTUdKaUxUUmlObVV0WWprM01DMWpOMkpqTUdNMU1XVTRNR1VRQVE9PRAHGiQ4ODBGQzg1OS0xNEUxLTRGNDYtOTQ1RS04QzM2M0VGQTZDNjg</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>MySQL</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Enterprise</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>lightweight</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" t="n">
-        <v>3.75</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Non-HA</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>asia-southeast1</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>10</v>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>HDD</t>
-        </is>
-      </c>
-      <c r="M4" t="n">
-        <v>5</v>
-      </c>
-      <c r="N4" t="n">
-        <v>350</v>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>hours</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>month</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>$54.20</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrT0RnNVpXSXlaaTFrTWpjd0xUUmhNRE10WW1Nd05TMDJNemhpTmpreE5HUTBaVEFRQVE9PRAHGiREQTc0NTNBMC0wQjhCLTQwMjItOERFMi04NTgyODVFRTMzOUM</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>$54.20</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1WkRBek1UUXlOQzB6WkdZMkxUUTBaV0l0WWpaa015MDRPREV6TUdNMU1qZGtNV1VRQVE9PRAHGiRCRDZDQ0M4NC1DNUEzLTQyNTktQTczNi0xRTUxM0ZBMUFDNkY</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>$54.20</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJsTVdRNFpXSTFaaTFpTUdKaUxUUmlObVV0WWprM01DMWpOMkpqTUdNMU1XVTRNR1VRQVE9PRAHGiQ3MUYxQzdENC1FMkExLTRGMTItQjk5Ni1DQTE5NzVDNjc1Q0I</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>PostgreSQL</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Enterprise</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>f1-micro</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>HA</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>asia-south1</t>
-        </is>
-      </c>
-      <c r="K5" t="n">
-        <v>11</v>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>HDD</t>
-        </is>
-      </c>
-      <c r="M5" t="n">
-        <v>5</v>
-      </c>
-      <c r="N5" t="n">
-        <v>730</v>
-      </c>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>$21.09</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrT0RnNVpXSXlaaTFrTWpjd0xUUmhNRE10WW1Nd05TMDJNemhpTmpreE5HUTBaVEFRQVE9PRAHGiRCRkRCOTc3My0xRDlGLTRCNzMtQkIxNy0wNERFNTU1NjBBMTc</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>$21.09</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1WkRBek1UUXlOQzB6WkdZMkxUUTBaV0l0WWpaa015MDRPREV6TUdNMU1qZGtNV1VRQVE9PRAHGiRDRkQxOTAzMS00ODY2LTQ2MzUtQkEyNS1FOTNDNTU1QkJGMkU</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>$21.09</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJsTVdRNFpXSTFaaTFpTUdKaUxUUmlObVV0WWprM01DMWpOMkpqTUdNMU1XVTRNR1VRQVE9PRAHGiQ1NjdFNDYxOS1DMjk1LTQxMDctOEUwQy0xQ0U2QTE0NzQ3NzA</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>PostgreSQL</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1.02</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Enterprise</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>STANDARD</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Non-HA</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>asia-southeast1</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>11</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>HDD</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>5</v>
-      </c>
-      <c r="N6" t="n">
-        <v>730</v>
-      </c>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>$139.04</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrT0RnNVpXSXlaaTFrTWpjd0xUUmhNRE10WW1Nd05TMDJNemhpTmpreE5HUTBaVEFRQVE9PRAHGiQ4MEVBQUJFMC0wNTJELTRCMkMtODRBQi1FRENBQkEwNDBDNjA</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>$104.75</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1WkRBek1UUXlOQzB6WkdZMkxUUTBaV0l0WWpaa015MDRPREV6TUdNMU1qZGtNV1VRQVE9PRAHGiQ5RTU0MTdDNy05RDE3LTRFMEItQTc0QS0zOTg5NjVFNDYyQzY</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>$67.72</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJsTVdRNFpXSTFaaTFpTUdKaUxUUmlObVV0WWprM01DMWpOMkpqTUdNMU1XVTRNR1VRQVE9PRAHGiRBOTJGMzhFNi0zOTVDLTQwMjEtODQ1Ny01RjFBMEE3NjBEQjk</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>PostgreSQL</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Enterprise</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>custom</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>8</v>
-      </c>
-      <c r="H7" t="n">
-        <v>52</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Non-HA</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>asia-south2</t>
-        </is>
-      </c>
-      <c r="K7" t="n">
-        <v>11</v>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>HDD</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>5</v>
-      </c>
-      <c r="N7" t="n">
-        <v>11</v>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>hours</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>month</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>$9.19</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJrT0RnNVpXSXlaaTFrTWpjd0xUUmhNRE10WW1Nd05TMDJNemhpTmpreE5HUTBaVEFRQVE9PRAHGiRGRDg2MjY3My03REJDLTQ0QzctODdDOS1BRkUzNDMwQTBEMDU</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>$9.19</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVE1WkRBek1UUXlOQzB6WkdZMkxUUTBaV0l0WWpaa015MDRPREV6TUdNMU1qZGtNV1VRQVE9PRAHGiQ5MzA4NEI3Ri0yMkEzLTRBNzEtQjAzNi1FNzAzRTQ5M0RCQTU</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>$9.19</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>https://cloud.google.com/products/calculator?dl=CjhDaVJsTVdRNFpXSTFaaTFpTUdKaUxUUmlObVV0WWprM01DMWpOMkpqTUdNMU1XVTRNR1VRQVE9PRAHGiRDRTg4QjZFOC02ODY5LTQzRUItOUM1OS01MEM5QTY0MjRDRkU</t>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>$812.23</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVF3TkdGa09UYzNNQzA0WVRrM0xUUXpaR1l0T0RFeU55MDFOemN4WVRNNE5HVmlOalFRQVE9PRAHGiQzNkQ3M0I3NS0wNjA5LTRGNkEtOTFEMC1DNDczNDdBMjBBOEE</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>$650.75</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVF5WkdWaVl6RmpaQzFrWXpnd0xUUTRZV1l0WW1ObU5pMDRObVJsTWpBM01tUXhaakFRQVE9PRAHGiQ3QkJGQzA1NC0yNERCLTQ5N0MtODBGMy1EODQ3NjExNTYyRjM</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>$476.36</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>https://cloud.google.com/products/calculator?dl=CjhDaVF6TW1GaE1qZG1PQzFtTVdObExUUmlNRE10WVRBellTMHhaRE15TjJObE9ESXhNamdRQVE9PRAHGiQ0QzRCRTYyMi02MTkwLTQ1OEEtQkU0My1FMkYxMjIwMDFBQkI</t>
         </is>
       </c>
     </row>

</xml_diff>